<commit_message>
Aggiunta energia interna alle tabelle
Agginti i dati relativi all'energia interna non presenti nelle tabelle usate in precedenza
</commit_message>
<xml_diff>
--- a/at.xlsx
+++ b/at.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Utenti\Lorenzo\Documents\Python\Projects\Tabell Fisica Tecnica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CCD416-16BE-4792-BFE6-BD561082057D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2657069-A0F2-4109-9FF7-EEE2AE888D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3060" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>t</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t>vv</t>
+  </si>
+  <si>
+    <t>ul</t>
+  </si>
+  <si>
+    <t>uvl</t>
+  </si>
+  <si>
+    <t>uv</t>
   </si>
   <si>
     <t>hl</t>
@@ -454,20 +463,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -496,2805 +505,3358 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.01</v>
       </c>
       <c r="B2">
-        <v>6.1119999999999989E-4</v>
+        <v>6.1170000000000007E-4</v>
       </c>
       <c r="C2">
         <v>1E-3</v>
       </c>
       <c r="D2">
-        <v>206.16200000000001</v>
+        <v>205.999</v>
       </c>
       <c r="E2">
-        <v>206.16300000000001</v>
+        <v>206</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>2501.6</v>
+        <v>2374.9</v>
       </c>
       <c r="H2">
-        <v>2501.6</v>
+        <v>2374.9</v>
       </c>
       <c r="I2">
+        <v>1E-3</v>
+      </c>
+      <c r="J2">
+        <v>2500.9</v>
+      </c>
+      <c r="K2">
+        <v>2500.9</v>
+      </c>
+      <c r="L2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>9.1575000000000006</v>
-      </c>
-      <c r="K2">
-        <v>9.1575000000000006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>9.1555999999999997</v>
+      </c>
+      <c r="N2">
+        <v>9.1555999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>7.0549999999999996E-4</v>
+        <v>8.7250000000000001E-4</v>
       </c>
       <c r="C3">
         <v>1E-3</v>
       </c>
       <c r="D3">
-        <v>179.922</v>
+        <v>147.029</v>
       </c>
       <c r="E3">
-        <v>179.923</v>
+        <v>147.03</v>
       </c>
       <c r="F3">
-        <v>8.4</v>
+        <v>21.018999999999998</v>
       </c>
       <c r="G3">
-        <v>2496.8000000000002</v>
+        <v>2360.8000000000002</v>
       </c>
       <c r="H3">
-        <v>2505.1999999999998</v>
+        <v>2381.8000000000002</v>
       </c>
       <c r="I3">
-        <v>3.0599999999999999E-2</v>
+        <v>21.02</v>
       </c>
       <c r="J3">
-        <v>9.0740999999999996</v>
+        <v>2489.1</v>
       </c>
       <c r="K3">
-        <v>9.1046999999999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2510.1</v>
+      </c>
+      <c r="L3">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="M3">
+        <v>8.9487000000000005</v>
+      </c>
+      <c r="N3">
+        <v>9.0249000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>8.1290000000000008E-4</v>
+        <v>1.2281E-3</v>
       </c>
       <c r="C4">
         <v>1E-3</v>
       </c>
       <c r="D4">
-        <v>157.27099999999999</v>
+        <v>106.319</v>
       </c>
       <c r="E4">
-        <v>157.27199999999999</v>
+        <v>106.32</v>
       </c>
       <c r="F4">
-        <v>16.8</v>
+        <v>42.02</v>
       </c>
       <c r="G4">
-        <v>2492.1</v>
+        <v>2346.6</v>
       </c>
       <c r="H4">
-        <v>2508.9</v>
+        <v>2388.6999999999998</v>
       </c>
       <c r="I4">
-        <v>6.1100000000000002E-2</v>
+        <v>42.021999999999998</v>
       </c>
       <c r="J4">
-        <v>8.9915000000000003</v>
+        <v>2477.1999999999998</v>
       </c>
       <c r="K4">
-        <v>9.0526</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2519.1999999999998</v>
+      </c>
+      <c r="L4">
+        <v>0.15110000000000001</v>
+      </c>
+      <c r="M4">
+        <v>8.7487999999999992</v>
+      </c>
+      <c r="N4">
+        <v>8.8999000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B5">
-        <v>9.3450000000000011E-4</v>
+        <v>1.7057000000000001E-3</v>
       </c>
       <c r="C5">
-        <v>1E-3</v>
+        <v>1.0009999999999999E-3</v>
       </c>
       <c r="D5">
-        <v>137.779</v>
+        <v>77.883999000000003</v>
       </c>
       <c r="E5">
-        <v>137.78</v>
+        <v>77.885000000000005</v>
       </c>
       <c r="F5">
-        <v>25.2</v>
+        <v>62.98</v>
       </c>
       <c r="G5">
-        <v>2487.4</v>
+        <v>2332.5</v>
       </c>
       <c r="H5">
-        <v>2512.6</v>
+        <v>2395.5</v>
       </c>
       <c r="I5">
-        <v>9.1300000000000006E-2</v>
+        <v>62.981999999999999</v>
       </c>
       <c r="J5">
-        <v>8.9101999999999997</v>
+        <v>2465.4</v>
       </c>
       <c r="K5">
-        <v>9.0015000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2528.3000000000002</v>
+      </c>
+      <c r="L5">
+        <v>0.22450000000000001</v>
+      </c>
+      <c r="M5">
+        <v>8.5558999999999994</v>
+      </c>
+      <c r="N5">
+        <v>8.7803000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B6">
-        <v>1.072E-3</v>
+        <v>2.3392E-3</v>
       </c>
       <c r="C6">
-        <v>1E-3</v>
+        <v>1.0020000000000001E-3</v>
       </c>
       <c r="D6">
-        <v>120.965</v>
+        <v>57.760998000000001</v>
       </c>
       <c r="E6">
-        <v>120.96599999999999</v>
+        <v>57.762</v>
       </c>
       <c r="F6">
-        <v>33.6</v>
+        <v>83.912999999999997</v>
       </c>
       <c r="G6">
-        <v>2482.6</v>
+        <v>2318.4</v>
       </c>
       <c r="H6">
-        <v>2516.1999999999998</v>
+        <v>2402.3000000000002</v>
       </c>
       <c r="I6">
-        <v>0.12130000000000001</v>
+        <v>83.915000000000006</v>
       </c>
       <c r="J6">
-        <v>8.83</v>
+        <v>2453.5</v>
       </c>
       <c r="K6">
-        <v>8.9512999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2537.4</v>
+      </c>
+      <c r="L6">
+        <v>0.29649999999999999</v>
+      </c>
+      <c r="M6">
+        <v>8.3696000000000002</v>
+      </c>
+      <c r="N6">
+        <v>8.6661000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B7">
-        <v>1.227E-3</v>
+        <v>3.1698E-3</v>
       </c>
       <c r="C7">
-        <v>1E-3</v>
+        <v>1.003E-3</v>
       </c>
       <c r="D7">
-        <v>106.429</v>
+        <v>43.338997000000013</v>
       </c>
       <c r="E7">
-        <v>106.43</v>
+        <v>43.34</v>
       </c>
       <c r="F7">
-        <v>42</v>
+        <v>104.83</v>
       </c>
       <c r="G7">
-        <v>2477.9</v>
+        <v>2304.3000000000002</v>
       </c>
       <c r="H7">
-        <v>2519.9</v>
+        <v>2409.1</v>
       </c>
       <c r="I7">
-        <v>0.151</v>
+        <v>104.83</v>
       </c>
       <c r="J7">
-        <v>8.7509999999999994</v>
+        <v>2441.6999999999998</v>
       </c>
       <c r="K7">
-        <v>8.9019999999999992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2546.5</v>
+      </c>
+      <c r="L7">
+        <v>0.36720000000000003</v>
+      </c>
+      <c r="M7">
+        <v>8.1895000000000007</v>
+      </c>
+      <c r="N7">
+        <v>8.5566999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B8">
-        <v>1.7139E-3</v>
+        <v>4.2469000000000014E-3</v>
       </c>
       <c r="C8">
-        <v>1.0009999999999999E-3</v>
+        <v>1.0039999999999999E-3</v>
       </c>
       <c r="D8">
-        <v>77.977000000000004</v>
+        <v>32.877996000000003</v>
       </c>
       <c r="E8">
-        <v>77.978000000000009</v>
+        <v>32.878999999999998</v>
       </c>
       <c r="F8">
-        <v>62.9</v>
+        <v>125.73</v>
       </c>
       <c r="G8">
-        <v>2466.1</v>
+        <v>2290.1999999999998</v>
       </c>
       <c r="H8">
-        <v>2529.1</v>
+        <v>2415.9</v>
       </c>
       <c r="I8">
-        <v>0.2243</v>
+        <v>125.74</v>
       </c>
       <c r="J8">
-        <v>8.5581999999999994</v>
+        <v>2429.8000000000002</v>
       </c>
       <c r="K8">
-        <v>8.7826000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2555.6</v>
+      </c>
+      <c r="L8">
+        <v>0.43680000000000002</v>
+      </c>
+      <c r="M8">
+        <v>8.0152000000000001</v>
+      </c>
+      <c r="N8">
+        <v>8.452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B9">
-        <v>2.3365999999999999E-3</v>
+        <v>5.6291000000000006E-3</v>
       </c>
       <c r="C9">
-        <v>1.0020000000000001E-3</v>
+        <v>1.0059999999999999E-3</v>
       </c>
       <c r="D9">
-        <v>57.837000000000003</v>
+        <v>25.203994000000002</v>
       </c>
       <c r="E9">
-        <v>57.838000000000001</v>
+        <v>25.204999999999998</v>
       </c>
       <c r="F9">
-        <v>83.9</v>
+        <v>146.63</v>
       </c>
       <c r="G9">
-        <v>2454.3000000000002</v>
+        <v>2276</v>
       </c>
       <c r="H9">
-        <v>2538.1999999999998</v>
+        <v>2422.6999999999998</v>
       </c>
       <c r="I9">
-        <v>0.29630000000000001</v>
+        <v>146.63999999999999</v>
       </c>
       <c r="J9">
-        <v>8.3720999999999997</v>
+        <v>2417.9</v>
       </c>
       <c r="K9">
-        <v>8.6684000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2564.6</v>
+      </c>
+      <c r="L9">
+        <v>0.50509999999999999</v>
+      </c>
+      <c r="M9">
+        <v>7.8465999999999996</v>
+      </c>
+      <c r="N9">
+        <v>8.3516999999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B10">
-        <v>3.166E-3</v>
+        <v>7.3851000000000003E-3</v>
       </c>
       <c r="C10">
-        <v>1.003E-3</v>
+        <v>1.008E-3</v>
       </c>
       <c r="D10">
-        <v>43.401000000000003</v>
+        <v>19.513991999999998</v>
       </c>
       <c r="E10">
-        <v>43.402000000000001</v>
+        <v>19.515000000000001</v>
       </c>
       <c r="F10">
-        <v>104.8</v>
+        <v>167.53</v>
       </c>
       <c r="G10">
-        <v>2442.5</v>
+        <v>2261.9</v>
       </c>
       <c r="H10">
-        <v>2547.3000000000002</v>
+        <v>2429.4</v>
       </c>
       <c r="I10">
-        <v>0.36699999999999999</v>
+        <v>167.53</v>
       </c>
       <c r="J10">
-        <v>8.1921999999999997</v>
+        <v>2406</v>
       </c>
       <c r="K10">
-        <v>8.5592000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2573.5</v>
+      </c>
+      <c r="L10">
+        <v>0.57240000000000002</v>
+      </c>
+      <c r="M10">
+        <v>7.6832000000000003</v>
+      </c>
+      <c r="N10">
+        <v>8.2555999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <v>4.2414999999999996E-3</v>
+        <v>9.5952999999999993E-3</v>
       </c>
       <c r="C11">
-        <v>1.0039999999999999E-3</v>
+        <v>1.01E-3</v>
       </c>
       <c r="D11">
-        <v>32.927999999999997</v>
+        <v>15.24999</v>
       </c>
       <c r="E11">
-        <v>32.929000000000002</v>
+        <v>15.250999999999999</v>
       </c>
       <c r="F11">
-        <v>125.7</v>
+        <v>188.43</v>
       </c>
       <c r="G11">
-        <v>2430.6999999999998</v>
+        <v>2247.6999999999998</v>
       </c>
       <c r="H11">
-        <v>2556.4</v>
+        <v>2436.1</v>
       </c>
       <c r="I11">
-        <v>0.4365</v>
+        <v>188.44</v>
       </c>
       <c r="J11">
-        <v>8.0181000000000004</v>
+        <v>2394</v>
       </c>
       <c r="K11">
-        <v>8.4545999999999992</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2582.4</v>
+      </c>
+      <c r="L11">
+        <v>0.63859999999999995</v>
+      </c>
+      <c r="M11">
+        <v>7.5247000000000002</v>
+      </c>
+      <c r="N11">
+        <v>8.1632999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B12">
-        <v>5.6215999999999992E-3</v>
+        <v>1.2352E-2</v>
       </c>
       <c r="C12">
-        <v>1.0059999999999999E-3</v>
+        <v>1.0120000000000001E-3</v>
       </c>
       <c r="D12">
-        <v>25.244</v>
+        <v>12.024988</v>
       </c>
       <c r="E12">
-        <v>25.245000000000001</v>
+        <v>12.026</v>
       </c>
       <c r="F12">
-        <v>146.6</v>
+        <v>209.33</v>
       </c>
       <c r="G12">
-        <v>2418.8000000000002</v>
+        <v>2233.4</v>
       </c>
       <c r="H12">
-        <v>2565.4</v>
+        <v>2442.6999999999998</v>
       </c>
       <c r="I12">
-        <v>0.50490000000000002</v>
+        <v>209.34</v>
       </c>
       <c r="J12">
-        <v>7.8494999999999999</v>
+        <v>2382</v>
       </c>
       <c r="K12">
-        <v>8.3543000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2591.3000000000002</v>
+      </c>
+      <c r="L12">
+        <v>0.70379999999999998</v>
+      </c>
+      <c r="M12">
+        <v>7.3710000000000004</v>
+      </c>
+      <c r="N12">
+        <v>8.0747999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B13">
-        <v>7.3749999999999996E-3</v>
+        <v>1.5762999999999999E-2</v>
       </c>
       <c r="C13">
-        <v>1.008E-3</v>
+        <v>1.0150000000000001E-3</v>
       </c>
       <c r="D13">
-        <v>19.545000000000002</v>
+        <v>9.5628849999999996</v>
       </c>
       <c r="E13">
-        <v>19.545999999999999</v>
+        <v>9.5639000000000003</v>
       </c>
       <c r="F13">
-        <v>167.5</v>
+        <v>230.24</v>
       </c>
       <c r="G13">
-        <v>2406.9</v>
+        <v>2219.1</v>
       </c>
       <c r="H13">
-        <v>2574.4</v>
+        <v>2449.3000000000002</v>
       </c>
       <c r="I13">
-        <v>0.57210000000000005</v>
+        <v>230.26</v>
       </c>
       <c r="J13">
-        <v>7.6860999999999997</v>
+        <v>2369.8000000000002</v>
       </c>
       <c r="K13">
-        <v>8.2583000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2600.1</v>
+      </c>
+      <c r="L13">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="M13">
+        <v>7.2218</v>
+      </c>
+      <c r="N13">
+        <v>7.9897999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B14">
-        <v>9.5820000000000002E-3</v>
+        <v>1.9946999999999999E-2</v>
       </c>
       <c r="C14">
-        <v>1.01E-3</v>
+        <v>1.0169999999999999E-3</v>
       </c>
       <c r="D14">
-        <v>15.275</v>
+        <v>7.6659829999999998</v>
       </c>
       <c r="E14">
-        <v>15.276</v>
+        <v>7.6669999999999998</v>
       </c>
       <c r="F14">
-        <v>188.4</v>
+        <v>251.16</v>
       </c>
       <c r="G14">
-        <v>2394.9</v>
+        <v>2204.6999999999998</v>
       </c>
       <c r="H14">
-        <v>2583.3000000000002</v>
+        <v>2455.9</v>
       </c>
       <c r="I14">
-        <v>0.63829999999999998</v>
+        <v>251.18</v>
       </c>
       <c r="J14">
-        <v>7.5277000000000003</v>
+        <v>2357.6999999999998</v>
       </c>
       <c r="K14">
-        <v>8.1661000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2608.8000000000002</v>
+      </c>
+      <c r="L14">
+        <v>0.83130000000000004</v>
+      </c>
+      <c r="M14">
+        <v>7.0769000000000002</v>
+      </c>
+      <c r="N14">
+        <v>7.9081999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B15">
-        <v>1.2335E-2</v>
+        <v>2.5042999999999999E-2</v>
       </c>
       <c r="C15">
-        <v>1.0120000000000001E-3</v>
+        <v>1.0200000000000001E-3</v>
       </c>
       <c r="D15">
-        <v>12.045</v>
+        <v>6.1924800000000007</v>
       </c>
       <c r="E15">
-        <v>12.045999999999999</v>
+        <v>6.1935000000000002</v>
       </c>
       <c r="F15">
-        <v>209.3</v>
+        <v>272.08999999999997</v>
       </c>
       <c r="G15">
-        <v>2382.9</v>
+        <v>2190.3000000000002</v>
       </c>
       <c r="H15">
-        <v>2592.1999999999998</v>
+        <v>2462.4</v>
       </c>
       <c r="I15">
-        <v>0.70350000000000001</v>
+        <v>272.12</v>
       </c>
       <c r="J15">
-        <v>7.3741000000000003</v>
+        <v>2345.4</v>
       </c>
       <c r="K15">
-        <v>8.0776000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2617.5</v>
+      </c>
+      <c r="L15">
+        <v>0.89370000000000005</v>
+      </c>
+      <c r="M15">
+        <v>6.9359999999999999</v>
+      </c>
+      <c r="N15">
+        <v>7.8296000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B16">
-        <v>1.5741000000000002E-2</v>
+        <v>3.1202000000000001E-2</v>
       </c>
       <c r="C16">
-        <v>1.0150000000000001E-3</v>
+        <v>1.023E-3</v>
       </c>
       <c r="D16">
-        <v>9.5778999999999996</v>
+        <v>5.0385770000000001</v>
       </c>
       <c r="E16">
-        <v>9.5789000000000009</v>
+        <v>5.0396000000000001</v>
       </c>
       <c r="F16">
-        <v>230.2</v>
+        <v>293.04000000000002</v>
       </c>
       <c r="G16">
-        <v>2370.8000000000002</v>
+        <v>2175.8000000000002</v>
       </c>
       <c r="H16">
-        <v>2601</v>
+        <v>2468.9</v>
       </c>
       <c r="I16">
-        <v>0.76770000000000005</v>
+        <v>293.07</v>
       </c>
       <c r="J16">
-        <v>7.2248000000000001</v>
+        <v>2333</v>
       </c>
       <c r="K16">
-        <v>7.9924999999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2626.1</v>
+      </c>
+      <c r="L16">
+        <v>0.95509999999999995</v>
+      </c>
+      <c r="M16">
+        <v>6.7988999999999997</v>
+      </c>
+      <c r="N16">
+        <v>7.7539999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B17">
-        <v>1.992E-2</v>
+        <v>3.8596999999999999E-2</v>
       </c>
       <c r="C17">
-        <v>1.0169999999999999E-3</v>
+        <v>1.026E-3</v>
       </c>
       <c r="D17">
-        <v>7.6775000000000002</v>
+        <v>4.1280739999999998</v>
       </c>
       <c r="E17">
-        <v>7.6784999999999997</v>
+        <v>4.1291000000000002</v>
       </c>
       <c r="F17">
-        <v>251.1</v>
+        <v>313.99</v>
       </c>
       <c r="G17">
-        <v>2358.6</v>
+        <v>2161.3000000000002</v>
       </c>
       <c r="H17">
-        <v>2609.6999999999998</v>
+        <v>2475.3000000000002</v>
       </c>
       <c r="I17">
-        <v>0.83099999999999996</v>
+        <v>314.02999999999997</v>
       </c>
       <c r="J17">
-        <v>7.0797999999999996</v>
+        <v>2320.6</v>
       </c>
       <c r="K17">
-        <v>7.9108000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2634.6</v>
+      </c>
+      <c r="L17">
+        <v>1.0158</v>
+      </c>
+      <c r="M17">
+        <v>6.6654999999999998</v>
+      </c>
+      <c r="N17">
+        <v>7.6811999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B18">
-        <v>2.5009E-2</v>
+        <v>4.7416E-2</v>
       </c>
       <c r="C18">
-        <v>1.0200000000000001E-3</v>
+        <v>1.029E-3</v>
       </c>
       <c r="D18">
-        <v>6.2012999999999998</v>
+        <v>3.404271</v>
       </c>
       <c r="E18">
-        <v>6.2023000000000001</v>
+        <v>3.4053</v>
       </c>
       <c r="F18">
-        <v>272</v>
+        <v>334.97</v>
       </c>
       <c r="G18">
-        <v>2346.3000000000002</v>
+        <v>2146.6</v>
       </c>
       <c r="H18">
-        <v>2618.4</v>
+        <v>2481.6</v>
       </c>
       <c r="I18">
-        <v>0.89329999999999998</v>
+        <v>335.02</v>
       </c>
       <c r="J18">
-        <v>6.9387999999999996</v>
+        <v>2308</v>
       </c>
       <c r="K18">
-        <v>7.8320999999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2643</v>
+      </c>
+      <c r="L18">
+        <v>1.0755999999999999</v>
+      </c>
+      <c r="M18">
+        <v>6.5354999999999999</v>
+      </c>
+      <c r="N18">
+        <v>7.6111000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="B19">
-        <v>3.1161999999999999E-2</v>
+        <v>5.7868000000000003E-2</v>
       </c>
       <c r="C19">
-        <v>1.023E-3</v>
+        <v>1.0319999999999999E-3</v>
       </c>
       <c r="D19">
-        <v>5.0453000000000001</v>
+        <v>2.8250679999999999</v>
       </c>
       <c r="E19">
-        <v>5.0462999999999996</v>
+        <v>2.8260999999999998</v>
       </c>
       <c r="F19">
-        <v>293</v>
+        <v>355.96</v>
       </c>
       <c r="G19">
-        <v>2334</v>
+        <v>2131.9</v>
       </c>
       <c r="H19">
-        <v>2626.9</v>
+        <v>2487.8000000000002</v>
       </c>
       <c r="I19">
-        <v>0.95479999999999998</v>
+        <v>356.02</v>
       </c>
       <c r="J19">
-        <v>6.8017000000000003</v>
+        <v>2295.3000000000002</v>
       </c>
       <c r="K19">
-        <v>7.7565</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2651.4</v>
+      </c>
+      <c r="L19">
+        <v>1.1346000000000001</v>
+      </c>
+      <c r="M19">
+        <v>6.4089</v>
+      </c>
+      <c r="N19">
+        <v>7.5434999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B20">
-        <v>3.8549E-2</v>
+        <v>7.0183000000000009E-2</v>
       </c>
       <c r="C20">
-        <v>1.026E-3</v>
+        <v>1.036E-3</v>
       </c>
       <c r="D20">
-        <v>4.1330999999999998</v>
+        <v>2.3582640000000001</v>
       </c>
       <c r="E20">
-        <v>4.1341000000000001</v>
+        <v>2.3593000000000002</v>
       </c>
       <c r="F20">
-        <v>313.89999999999998</v>
+        <v>376.97</v>
       </c>
       <c r="G20">
-        <v>2321.5</v>
+        <v>2117</v>
       </c>
       <c r="H20">
-        <v>2635.4</v>
+        <v>2494</v>
       </c>
       <c r="I20">
-        <v>1.0154000000000001</v>
+        <v>377.04</v>
       </c>
       <c r="J20">
-        <v>6.6680999999999999</v>
+        <v>2282.5</v>
       </c>
       <c r="K20">
-        <v>7.6835000000000004</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2659.6</v>
+      </c>
+      <c r="L20">
+        <v>1.1929000000000001</v>
+      </c>
+      <c r="M20">
+        <v>6.2853000000000003</v>
+      </c>
+      <c r="N20">
+        <v>7.4782000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="B21">
-        <v>4.7359999999999999E-2</v>
+        <v>8.460899999999999E-2</v>
       </c>
       <c r="C21">
-        <v>1.029E-3</v>
+        <v>1.0399999999999999E-3</v>
       </c>
       <c r="D21">
-        <v>3.4081000000000001</v>
+        <v>1.97976</v>
       </c>
       <c r="E21">
-        <v>3.4091</v>
+        <v>1.9807999999999999</v>
       </c>
       <c r="F21">
-        <v>334.9</v>
+        <v>398</v>
       </c>
       <c r="G21">
-        <v>2308.8000000000002</v>
+        <v>2102</v>
       </c>
       <c r="H21">
-        <v>2643.8</v>
+        <v>2500.1</v>
       </c>
       <c r="I21">
-        <v>1.0752999999999999</v>
+        <v>398.09</v>
       </c>
       <c r="J21">
-        <v>6.5380000000000003</v>
+        <v>2269.6</v>
       </c>
       <c r="K21">
-        <v>7.6132999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2667.6</v>
+      </c>
+      <c r="L21">
+        <v>1.2504</v>
+      </c>
+      <c r="M21">
+        <v>6.1646999999999998</v>
+      </c>
+      <c r="N21">
+        <v>7.4150999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B22">
-        <v>5.7803000000000007E-2</v>
+        <v>0.10142</v>
       </c>
       <c r="C22">
-        <v>1.0330000000000001E-3</v>
+        <v>1.0430000000000001E-3</v>
       </c>
       <c r="D22">
-        <v>2.8277999999999999</v>
+        <v>1.670957</v>
       </c>
       <c r="E22">
-        <v>2.8288000000000002</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="F22">
-        <v>355.9</v>
+        <v>419.06</v>
       </c>
       <c r="G22">
-        <v>2296.1</v>
+        <v>2087</v>
       </c>
       <c r="H22">
-        <v>2652</v>
+        <v>2506</v>
       </c>
       <c r="I22">
-        <v>1.1343000000000001</v>
+        <v>419.17</v>
       </c>
       <c r="J22">
-        <v>6.4111000000000002</v>
+        <v>2256.4</v>
       </c>
       <c r="K22">
-        <v>7.5453999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2675.6</v>
+      </c>
+      <c r="L22">
+        <v>1.3071999999999999</v>
+      </c>
+      <c r="M22">
+        <v>6.0469999999999997</v>
+      </c>
+      <c r="N22">
+        <v>7.3541999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B23">
-        <v>7.0109000000000005E-2</v>
+        <v>0.12089999999999999</v>
       </c>
       <c r="C23">
-        <v>1.036E-3</v>
+        <v>1.047E-3</v>
       </c>
       <c r="D23">
-        <v>2.3603000000000001</v>
+        <v>1.4175530000000001</v>
       </c>
       <c r="E23">
-        <v>2.3613</v>
+        <v>1.4186000000000001</v>
       </c>
       <c r="F23">
-        <v>376.9</v>
+        <v>440.15</v>
       </c>
       <c r="G23">
-        <v>2283.1999999999998</v>
+        <v>2071.8000000000002</v>
       </c>
       <c r="H23">
-        <v>2660.1</v>
+        <v>2511.9</v>
       </c>
       <c r="I23">
-        <v>1.1924999999999999</v>
+        <v>440.28</v>
       </c>
       <c r="J23">
-        <v>6.2873000000000001</v>
+        <v>2243.1</v>
       </c>
       <c r="K23">
-        <v>7.4798</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2683.4</v>
+      </c>
+      <c r="L23">
+        <v>1.3633999999999999</v>
+      </c>
+      <c r="M23">
+        <v>5.9318999999999997</v>
+      </c>
+      <c r="N23">
+        <v>7.2952000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B24">
-        <v>8.4526000000000004E-2</v>
+        <v>0.14338000000000001</v>
       </c>
       <c r="C24">
-        <v>1.0399999999999999E-3</v>
+        <v>1.052E-3</v>
       </c>
       <c r="D24">
-        <v>1.9812000000000001</v>
+        <v>1.208348</v>
       </c>
       <c r="E24">
-        <v>1.9822</v>
+        <v>1.2094</v>
       </c>
       <c r="F24">
-        <v>398</v>
+        <v>461.27</v>
       </c>
       <c r="G24">
-        <v>2270.1999999999998</v>
+        <v>2056.4</v>
       </c>
       <c r="H24">
-        <v>2668.1</v>
+        <v>2517.6999999999998</v>
       </c>
       <c r="I24">
-        <v>1.2501</v>
+        <v>461.42</v>
       </c>
       <c r="J24">
-        <v>6.1665000000000001</v>
+        <v>2229.6999999999998</v>
       </c>
       <c r="K24">
-        <v>7.4165999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2691.1</v>
+      </c>
+      <c r="L24">
+        <v>1.4188000000000001</v>
+      </c>
+      <c r="M24">
+        <v>5.8193000000000001</v>
+      </c>
+      <c r="N24">
+        <v>7.2382</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="B25">
-        <v>0.101325</v>
+        <v>0.16918</v>
       </c>
       <c r="C25">
-        <v>1.044E-3</v>
+        <v>1.0560000000000001E-3</v>
       </c>
       <c r="D25">
-        <v>1.6719999999999999</v>
+        <v>1.0349440000000001</v>
       </c>
       <c r="E25">
-        <v>1.673</v>
+        <v>1.036</v>
       </c>
       <c r="F25">
-        <v>419.1</v>
+        <v>482.42</v>
       </c>
       <c r="G25">
-        <v>2256.9</v>
+        <v>2040.9</v>
       </c>
       <c r="H25">
-        <v>2676</v>
+        <v>2523.3000000000002</v>
       </c>
       <c r="I25">
-        <v>1.3069</v>
+        <v>482.59</v>
       </c>
       <c r="J25">
-        <v>6.0484999999999998</v>
+        <v>2216</v>
       </c>
       <c r="K25">
-        <v>7.3554000000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2698.6</v>
+      </c>
+      <c r="L25">
+        <v>1.4737</v>
+      </c>
+      <c r="M25">
+        <v>5.7092000000000001</v>
+      </c>
+      <c r="N25">
+        <v>7.1829000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B26">
-        <v>0.1208</v>
+        <v>0.19867000000000001</v>
       </c>
       <c r="C26">
-        <v>1.0480000000000001E-3</v>
+        <v>1.06E-3</v>
       </c>
       <c r="D26">
-        <v>1.4182999999999999</v>
+        <v>0.89027000000000001</v>
       </c>
       <c r="E26">
-        <v>1.4193</v>
+        <v>0.89132999999999996</v>
       </c>
       <c r="F26">
-        <v>440.2</v>
+        <v>503.6</v>
       </c>
       <c r="G26">
-        <v>2243.6</v>
+        <v>2025.3</v>
       </c>
       <c r="H26">
-        <v>2683.7</v>
+        <v>2528.9</v>
       </c>
       <c r="I26">
-        <v>1.363</v>
+        <v>503.81</v>
       </c>
       <c r="J26">
-        <v>5.9330999999999996</v>
+        <v>2202.1</v>
       </c>
       <c r="K26">
-        <v>7.2961999999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2706</v>
+      </c>
+      <c r="L26">
+        <v>1.5279</v>
+      </c>
+      <c r="M26">
+        <v>5.6013000000000002</v>
+      </c>
+      <c r="N26">
+        <v>7.1292</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B27">
-        <v>0.14327000000000001</v>
+        <v>0.23222999999999999</v>
       </c>
       <c r="C27">
-        <v>1.052E-3</v>
+        <v>1.065E-3</v>
       </c>
       <c r="D27">
-        <v>1.2089000000000001</v>
+        <v>0.76905500000000004</v>
       </c>
       <c r="E27">
-        <v>1.2099</v>
+        <v>0.77012000000000003</v>
       </c>
       <c r="F27">
-        <v>461.3</v>
+        <v>524.83000000000004</v>
       </c>
       <c r="G27">
-        <v>2230</v>
+        <v>2009.5</v>
       </c>
       <c r="H27">
-        <v>2691.3</v>
+        <v>2534.3000000000002</v>
       </c>
       <c r="I27">
-        <v>1.4185000000000001</v>
+        <v>525.07000000000005</v>
       </c>
       <c r="J27">
-        <v>5.8202999999999996</v>
+        <v>2188.1</v>
       </c>
       <c r="K27">
-        <v>7.2388000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2713.1</v>
+      </c>
+      <c r="L27">
+        <v>1.5815999999999999</v>
+      </c>
+      <c r="M27">
+        <v>5.4955999999999996</v>
+      </c>
+      <c r="N27">
+        <v>7.0770999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B28">
-        <v>0.16905999999999999</v>
+        <v>0.27028000000000002</v>
       </c>
       <c r="C28">
-        <v>1.0560000000000001E-3</v>
+        <v>1.07E-3</v>
       </c>
       <c r="D28">
-        <v>1.0353000000000001</v>
+        <v>0.66700999999999999</v>
       </c>
       <c r="E28">
-        <v>1.0363</v>
+        <v>0.66808000000000001</v>
       </c>
       <c r="F28">
-        <v>482.5</v>
+        <v>546.1</v>
       </c>
       <c r="G28">
-        <v>2216.1999999999998</v>
+        <v>1993.4</v>
       </c>
       <c r="H28">
-        <v>2698.7</v>
+        <v>2539.5</v>
       </c>
       <c r="I28">
-        <v>1.4733000000000001</v>
+        <v>546.38</v>
       </c>
       <c r="J28">
-        <v>5.7099000000000002</v>
+        <v>2173.6999999999998</v>
       </c>
       <c r="K28">
-        <v>7.1832000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2720.1</v>
+      </c>
+      <c r="L28">
+        <v>1.6346000000000001</v>
+      </c>
+      <c r="M28">
+        <v>5.3918999999999997</v>
+      </c>
+      <c r="N28">
+        <v>7.0265000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="B29">
-        <v>0.19853999999999999</v>
+        <v>0.31322000000000011</v>
       </c>
       <c r="C29">
-        <v>1.0610000000000001E-3</v>
+        <v>1.075E-3</v>
       </c>
       <c r="D29">
-        <v>0.89046000000000003</v>
+        <v>0.58071499999999998</v>
       </c>
       <c r="E29">
-        <v>0.89152000000000009</v>
+        <v>0.58179000000000003</v>
       </c>
       <c r="F29">
-        <v>503.7</v>
+        <v>567.41</v>
       </c>
       <c r="G29">
-        <v>2202.1999999999998</v>
+        <v>1977.3</v>
       </c>
       <c r="H29">
-        <v>2706</v>
+        <v>2544.6999999999998</v>
       </c>
       <c r="I29">
-        <v>1.5276000000000001</v>
+        <v>567.75</v>
       </c>
       <c r="J29">
-        <v>5.6017000000000001</v>
+        <v>2159.1</v>
       </c>
       <c r="K29">
-        <v>7.1292999999999997</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2726.9</v>
+      </c>
+      <c r="L29">
+        <v>1.6872</v>
+      </c>
+      <c r="M29">
+        <v>5.2900999999999998</v>
+      </c>
+      <c r="N29">
+        <v>6.9772999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="B30">
-        <v>0.2321</v>
+        <v>0.36153000000000002</v>
       </c>
       <c r="C30">
-        <v>1.065E-3</v>
+        <v>1.08E-3</v>
       </c>
       <c r="D30">
-        <v>0.76917000000000002</v>
+        <v>0.50741999999999998</v>
       </c>
       <c r="E30">
-        <v>0.77022999999999997</v>
+        <v>0.50849999999999995</v>
       </c>
       <c r="F30">
-        <v>525</v>
+        <v>588.77</v>
       </c>
       <c r="G30">
-        <v>2188</v>
+        <v>1960.9</v>
       </c>
       <c r="H30">
-        <v>2713</v>
+        <v>2549.6</v>
       </c>
       <c r="I30">
-        <v>1.5812999999999999</v>
+        <v>589.16</v>
       </c>
       <c r="J30">
-        <v>5.4957000000000003</v>
+        <v>2144.3000000000002</v>
       </c>
       <c r="K30">
-        <v>7.0769000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2733.5</v>
+      </c>
+      <c r="L30">
+        <v>1.7392000000000001</v>
+      </c>
+      <c r="M30">
+        <v>5.1901000000000002</v>
+      </c>
+      <c r="N30">
+        <v>6.9294000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="B31">
-        <v>0.27012999999999998</v>
+        <v>0.41567999999999999</v>
       </c>
       <c r="C31">
-        <v>1.07E-3</v>
+        <v>1.085E-3</v>
       </c>
       <c r="D31">
-        <v>0.66706999999999994</v>
+        <v>0.444915</v>
       </c>
       <c r="E31">
-        <v>0.66813999999999996</v>
+        <v>0.44600000000000001</v>
       </c>
       <c r="F31">
-        <v>546.29999999999995</v>
+        <v>610.19000000000005</v>
       </c>
       <c r="G31">
-        <v>2173.6</v>
+        <v>1944.2</v>
       </c>
       <c r="H31">
-        <v>2719.9</v>
+        <v>2554.4</v>
       </c>
       <c r="I31">
-        <v>1.6344000000000001</v>
+        <v>610.64</v>
       </c>
       <c r="J31">
-        <v>5.3917000000000002</v>
+        <v>2129.1999999999998</v>
       </c>
       <c r="K31">
-        <v>7.0260999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2739.8</v>
+      </c>
+      <c r="L31">
+        <v>1.7907999999999999</v>
+      </c>
+      <c r="M31">
+        <v>5.0918999999999999</v>
+      </c>
+      <c r="N31">
+        <v>6.8826999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="B32">
-        <v>0.31308000000000002</v>
+        <v>0.47616000000000003</v>
       </c>
       <c r="C32">
-        <v>1.075E-3</v>
+        <v>1.091E-3</v>
       </c>
       <c r="D32">
-        <v>0.58073999999999992</v>
+        <v>0.39138899999999999</v>
       </c>
       <c r="E32">
-        <v>0.58181000000000005</v>
+        <v>0.39248</v>
       </c>
       <c r="F32">
-        <v>567.70000000000005</v>
+        <v>631.66</v>
       </c>
       <c r="G32">
-        <v>2158.9</v>
+        <v>1927.4</v>
       </c>
       <c r="H32">
-        <v>2726.6</v>
+        <v>2559.1</v>
       </c>
       <c r="I32">
-        <v>1.6869000000000001</v>
+        <v>632.17999999999995</v>
       </c>
       <c r="J32">
-        <v>5.2896999999999998</v>
+        <v>2113.8000000000002</v>
       </c>
       <c r="K32">
-        <v>6.9766000000000004</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2745.9</v>
+      </c>
+      <c r="L32">
+        <v>1.8418000000000001</v>
+      </c>
+      <c r="M32">
+        <v>4.9953000000000003</v>
+      </c>
+      <c r="N32">
+        <v>6.8371000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="B33">
-        <v>0.36137999999999998</v>
+        <v>0.54349000000000003</v>
       </c>
       <c r="C33">
-        <v>1.08E-3</v>
+        <v>1.096E-3</v>
       </c>
       <c r="D33">
-        <v>0.50741000000000003</v>
+        <v>0.34538400000000002</v>
       </c>
       <c r="E33">
-        <v>0.50849</v>
+        <v>0.34648000000000001</v>
       </c>
       <c r="F33">
-        <v>589.1</v>
+        <v>653.19000000000005</v>
       </c>
       <c r="G33">
-        <v>2144</v>
+        <v>1910.3</v>
       </c>
       <c r="H33">
-        <v>2733.1</v>
+        <v>2563.5</v>
       </c>
       <c r="I33">
-        <v>1.7390000000000001</v>
+        <v>653.79</v>
       </c>
       <c r="J33">
-        <v>5.1894</v>
+        <v>2098</v>
       </c>
       <c r="K33">
-        <v>6.9283999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2751.8</v>
+      </c>
+      <c r="L33">
+        <v>1.8924000000000001</v>
+      </c>
+      <c r="M33">
+        <v>4.9001999999999999</v>
+      </c>
+      <c r="N33">
+        <v>6.7927</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B34">
-        <v>0.41552</v>
+        <v>0.61823000000000006</v>
       </c>
       <c r="C34">
-        <v>1.085E-3</v>
+        <v>1.1019999999999999E-3</v>
       </c>
       <c r="D34">
-        <v>0.44489000000000001</v>
+        <v>0.30569800000000003</v>
       </c>
       <c r="E34">
-        <v>0.44596999999999998</v>
+        <v>0.30680000000000002</v>
       </c>
       <c r="F34">
-        <v>610.6</v>
+        <v>674.79</v>
       </c>
       <c r="G34">
-        <v>2128.6999999999998</v>
+        <v>1893</v>
       </c>
       <c r="H34">
-        <v>2739.3</v>
+        <v>2567.8000000000002</v>
       </c>
       <c r="I34">
-        <v>1.7906</v>
+        <v>675.47</v>
       </c>
       <c r="J34">
-        <v>5.0910000000000002</v>
+        <v>2082</v>
       </c>
       <c r="K34">
-        <v>6.8815</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2757.5</v>
+      </c>
+      <c r="L34">
+        <v>1.9426000000000001</v>
+      </c>
+      <c r="M34">
+        <v>4.8066000000000004</v>
+      </c>
+      <c r="N34">
+        <v>6.7492000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="B35">
-        <v>0.47599999999999998</v>
+        <v>0.70092999999999994</v>
       </c>
       <c r="C35">
-        <v>1.091E-3</v>
+        <v>1.108E-3</v>
       </c>
       <c r="D35">
-        <v>0.39135999999999999</v>
+        <v>0.27133200000000002</v>
       </c>
       <c r="E35">
-        <v>0.39245000000000002</v>
+        <v>0.27244000000000002</v>
       </c>
       <c r="F35">
-        <v>632.1</v>
+        <v>696.46</v>
       </c>
       <c r="G35">
-        <v>2113.1999999999998</v>
+        <v>1875.4</v>
       </c>
       <c r="H35">
-        <v>2745.4</v>
+        <v>2571.9</v>
       </c>
       <c r="I35">
-        <v>1.8415999999999999</v>
+        <v>697.24</v>
       </c>
       <c r="J35">
-        <v>4.9941000000000004</v>
+        <v>2065.6</v>
       </c>
       <c r="K35">
-        <v>6.8357999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2762.8</v>
+      </c>
+      <c r="L35">
+        <v>1.9923</v>
+      </c>
+      <c r="M35">
+        <v>4.7142999999999997</v>
+      </c>
+      <c r="N35">
+        <v>6.7066999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B36">
-        <v>0.54332999999999998</v>
+        <v>0.79218</v>
       </c>
       <c r="C36">
-        <v>1.096E-3</v>
+        <v>1.114E-3</v>
       </c>
       <c r="D36">
-        <v>0.34555000000000002</v>
+        <v>0.24148600000000001</v>
       </c>
       <c r="E36">
-        <v>0.34644000000000003</v>
+        <v>0.24260000000000001</v>
       </c>
       <c r="F36">
-        <v>653.79999999999995</v>
+        <v>718.2</v>
       </c>
       <c r="G36">
-        <v>2097.4</v>
+        <v>1857.5</v>
       </c>
       <c r="H36">
-        <v>2751.2</v>
+        <v>2575.6999999999998</v>
       </c>
       <c r="I36">
-        <v>1.8923000000000001</v>
+        <v>719.08</v>
       </c>
       <c r="J36">
-        <v>4.8989000000000003</v>
+        <v>2048.8000000000002</v>
       </c>
       <c r="K36">
-        <v>6.7911000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2767.9</v>
+      </c>
+      <c r="L36">
+        <v>2.0417000000000001</v>
+      </c>
+      <c r="M36">
+        <v>4.6233000000000004</v>
+      </c>
+      <c r="N36">
+        <v>6.665</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="B37">
-        <v>0.61806000000000005</v>
+        <v>0.89260000000000006</v>
       </c>
       <c r="C37">
-        <v>1.1019999999999999E-3</v>
+        <v>1.121E-3</v>
       </c>
       <c r="D37">
-        <v>0.30565999999999999</v>
+        <v>0.21546899999999999</v>
       </c>
       <c r="E37">
-        <v>0.30675999999999998</v>
+        <v>0.21659</v>
       </c>
       <c r="F37">
-        <v>675.5</v>
+        <v>740.02</v>
       </c>
       <c r="G37">
-        <v>2081.3000000000002</v>
+        <v>1839.4</v>
       </c>
       <c r="H37">
-        <v>2756.7</v>
+        <v>2579.4</v>
       </c>
       <c r="I37">
-        <v>1.9424999999999999</v>
+        <v>741.02</v>
       </c>
       <c r="J37">
-        <v>4.8049999999999997</v>
+        <v>2031.7</v>
       </c>
       <c r="K37">
-        <v>6.7473000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2772.7</v>
+      </c>
+      <c r="L37">
+        <v>2.0905999999999998</v>
+      </c>
+      <c r="M37">
+        <v>4.5335000000000001</v>
+      </c>
+      <c r="N37">
+        <v>6.6242000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="B38">
-        <v>0.70077</v>
+        <v>1.0027999999999999</v>
       </c>
       <c r="C38">
-        <v>1.108E-3</v>
+        <v>1.127E-3</v>
       </c>
       <c r="D38">
-        <v>0.27128999999999998</v>
+        <v>0.192713</v>
       </c>
       <c r="E38">
-        <v>0.27239999999999998</v>
+        <v>0.19384000000000001</v>
       </c>
       <c r="F38">
-        <v>697.3</v>
+        <v>761.92</v>
       </c>
       <c r="G38">
-        <v>2064.8000000000002</v>
+        <v>1820.9</v>
       </c>
       <c r="H38">
-        <v>2762</v>
+        <v>2582.8000000000002</v>
       </c>
       <c r="I38">
-        <v>1.9923</v>
+        <v>763.05</v>
       </c>
       <c r="J38">
-        <v>4.7126000000000001</v>
+        <v>2014.2</v>
       </c>
       <c r="K38">
-        <v>6.7047999999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2777.2</v>
+      </c>
+      <c r="L38">
+        <v>2.1392000000000002</v>
+      </c>
+      <c r="M38">
+        <v>4.4447999999999999</v>
+      </c>
+      <c r="N38">
+        <v>6.5841000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="B39">
-        <v>0.79202000000000006</v>
+        <v>1.1234999999999999</v>
       </c>
       <c r="C39">
-        <v>1.1150000000000001E-3</v>
+        <v>1.134E-3</v>
       </c>
       <c r="D39">
-        <v>0.24143999999999999</v>
+        <v>0.172766</v>
       </c>
       <c r="E39">
-        <v>0.24254999999999999</v>
+        <v>0.1739</v>
       </c>
       <c r="F39">
-        <v>719.1</v>
+        <v>783.91</v>
       </c>
       <c r="G39">
-        <v>2047.9</v>
+        <v>1802.1</v>
       </c>
       <c r="H39">
-        <v>2767.1</v>
+        <v>2586</v>
       </c>
       <c r="I39">
-        <v>2.0415999999999999</v>
+        <v>785.19</v>
       </c>
       <c r="J39">
-        <v>4.6214000000000004</v>
+        <v>1996.2</v>
       </c>
       <c r="K39">
-        <v>6.6630000000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2781.4</v>
+      </c>
+      <c r="L39">
+        <v>2.1875</v>
+      </c>
+      <c r="M39">
+        <v>4.3571999999999997</v>
+      </c>
+      <c r="N39">
+        <v>6.5446999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B40">
-        <v>0.89244000000000001</v>
+        <v>1.2552000000000001</v>
       </c>
       <c r="C40">
-        <v>1.121E-3</v>
+        <v>1.1410000000000001E-3</v>
       </c>
       <c r="D40">
-        <v>0.21542</v>
+        <v>0.155219</v>
       </c>
       <c r="E40">
-        <v>0.21654000000000001</v>
+        <v>0.15636</v>
       </c>
       <c r="F40">
-        <v>741.1</v>
+        <v>806</v>
       </c>
       <c r="G40">
-        <v>2030.7</v>
+        <v>1783</v>
       </c>
       <c r="H40">
-        <v>2771.8</v>
+        <v>2589</v>
       </c>
       <c r="I40">
-        <v>2.0905999999999998</v>
+        <v>807.43</v>
       </c>
       <c r="J40">
-        <v>4.5313999999999997</v>
+        <v>1977.9</v>
       </c>
       <c r="K40">
-        <v>6.6220999999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2785.3</v>
+      </c>
+      <c r="L40">
+        <v>2.2355</v>
+      </c>
+      <c r="M40">
+        <v>4.2705000000000002</v>
+      </c>
+      <c r="N40">
+        <v>6.5058999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B41">
-        <v>1.0026999999999999</v>
+        <v>1.3988</v>
       </c>
       <c r="C41">
-        <v>1.1280000000000001E-3</v>
+        <v>1.1490000000000001E-3</v>
       </c>
       <c r="D41">
-        <v>0.19267000000000001</v>
+        <v>0.139741</v>
       </c>
       <c r="E41">
-        <v>0.1938</v>
+        <v>0.14088999999999999</v>
       </c>
       <c r="F41">
-        <v>763.1</v>
+        <v>828.18</v>
       </c>
       <c r="G41">
-        <v>2013.2</v>
+        <v>1763.6</v>
       </c>
       <c r="H41">
-        <v>2776.3</v>
+        <v>2591.6999999999998</v>
       </c>
       <c r="I41">
-        <v>2.1393</v>
+        <v>829.78</v>
       </c>
       <c r="J41">
-        <v>4.4425999999999997</v>
+        <v>1959</v>
       </c>
       <c r="K41">
-        <v>6.5819000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2788.8</v>
+      </c>
+      <c r="L41">
+        <v>2.2831000000000001</v>
+      </c>
+      <c r="M41">
+        <v>4.1847000000000003</v>
+      </c>
+      <c r="N41">
+        <v>6.4678000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="B42">
-        <v>1.1233</v>
+        <v>1.5548999999999999</v>
       </c>
       <c r="C42">
-        <v>1.134E-3</v>
+        <v>1.157E-3</v>
       </c>
       <c r="D42">
-        <v>0.17263000000000001</v>
+        <v>0.126053</v>
       </c>
       <c r="E42">
-        <v>0.17385999999999999</v>
+        <v>0.12720999999999999</v>
       </c>
       <c r="F42">
-        <v>785.3</v>
+        <v>850.46</v>
       </c>
       <c r="G42">
-        <v>1995.2</v>
+        <v>1743.7</v>
       </c>
       <c r="H42">
-        <v>2780.4</v>
+        <v>2594.1999999999998</v>
       </c>
       <c r="I42">
-        <v>2.1876000000000002</v>
+        <v>852.26</v>
       </c>
       <c r="J42">
-        <v>4.3548</v>
+        <v>1939.8</v>
       </c>
       <c r="K42">
-        <v>6.5423999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2792</v>
+      </c>
+      <c r="L42">
+        <v>2.3304999999999998</v>
+      </c>
+      <c r="M42">
+        <v>4.0997000000000003</v>
+      </c>
+      <c r="N42">
+        <v>6.4302000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="B43">
-        <v>1.2551000000000001</v>
+        <v>1.7242999999999999</v>
       </c>
       <c r="C43">
-        <v>1.142E-3</v>
+        <v>1.1640000000000001E-3</v>
       </c>
       <c r="D43">
-        <v>0.15518000000000001</v>
+        <v>0.113916</v>
       </c>
       <c r="E43">
-        <v>0.15631999999999999</v>
+        <v>0.11508</v>
       </c>
       <c r="F43">
-        <v>807.5</v>
+        <v>872.86</v>
       </c>
       <c r="G43">
-        <v>1976.7</v>
+        <v>1723.5</v>
       </c>
       <c r="H43">
-        <v>2784.3</v>
+        <v>2596.4</v>
       </c>
       <c r="I43">
-        <v>2.2355999999999998</v>
+        <v>874.87</v>
       </c>
       <c r="J43">
-        <v>4.2679999999999998</v>
+        <v>1920</v>
       </c>
       <c r="K43">
-        <v>6.5035999999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2794.8</v>
+      </c>
+      <c r="L43">
+        <v>2.3776000000000002</v>
+      </c>
+      <c r="M43">
+        <v>4.0153999999999996</v>
+      </c>
+      <c r="N43">
+        <v>6.3929999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="B44">
-        <v>1.3987000000000001</v>
+        <v>1.9077</v>
       </c>
       <c r="C44">
-        <v>1.1490000000000001E-3</v>
+        <v>1.173E-3</v>
       </c>
       <c r="D44">
-        <v>0.13969000000000001</v>
+        <v>0.103117</v>
       </c>
       <c r="E44">
-        <v>0.14083999999999999</v>
+        <v>0.10428999999999999</v>
       </c>
       <c r="F44">
-        <v>829.9</v>
+        <v>895.38</v>
       </c>
       <c r="G44">
-        <v>1957.9</v>
+        <v>1702.9</v>
       </c>
       <c r="H44">
-        <v>2787.8</v>
+        <v>2598.3000000000002</v>
       </c>
       <c r="I44">
-        <v>2.2833000000000001</v>
+        <v>897.61</v>
       </c>
       <c r="J44">
-        <v>4.1821000000000002</v>
+        <v>1899.7</v>
       </c>
       <c r="K44">
-        <v>6.4653999999999998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2797.3</v>
+      </c>
+      <c r="L44">
+        <v>2.4245000000000001</v>
+      </c>
+      <c r="M44">
+        <v>3.9318</v>
+      </c>
+      <c r="N44">
+        <v>6.3563000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="B45">
-        <v>1.5548999999999999</v>
+        <v>2.1059000000000001</v>
       </c>
       <c r="C45">
-        <v>1.157E-3</v>
+        <v>1.181E-3</v>
       </c>
       <c r="D45">
-        <v>0.12601000000000001</v>
+        <v>9.3498999999999999E-2</v>
       </c>
       <c r="E45">
-        <v>0.12716</v>
+        <v>9.468E-2</v>
       </c>
       <c r="F45">
-        <v>852.4</v>
+        <v>918.02</v>
       </c>
       <c r="G45">
-        <v>1938.6</v>
+        <v>1681.9</v>
       </c>
       <c r="H45">
-        <v>2790.9</v>
+        <v>2599.9</v>
       </c>
       <c r="I45">
-        <v>2.3307000000000002</v>
+        <v>920.5</v>
       </c>
       <c r="J45">
-        <v>4.0971000000000002</v>
+        <v>1878.8</v>
       </c>
       <c r="K45">
-        <v>6.4278000000000004</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2799.3</v>
+      </c>
+      <c r="L45">
+        <v>2.4712000000000001</v>
+      </c>
+      <c r="M45">
+        <v>3.8489</v>
+      </c>
+      <c r="N45">
+        <v>6.32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="B46">
-        <v>1.7242999999999999</v>
+        <v>2.3195999999999999</v>
       </c>
       <c r="C46">
-        <v>1.1640000000000001E-3</v>
+        <v>1.1900000000000001E-3</v>
       </c>
       <c r="D46">
-        <v>0.11387</v>
+        <v>8.4904000000000007E-2</v>
       </c>
       <c r="E46">
-        <v>0.11502999999999999</v>
+        <v>8.6094000000000004E-2</v>
       </c>
       <c r="F46">
-        <v>875</v>
+        <v>940.79</v>
       </c>
       <c r="G46">
-        <v>1918.8</v>
+        <v>1660.5</v>
       </c>
       <c r="H46">
-        <v>2793.8</v>
+        <v>2601.3000000000002</v>
       </c>
       <c r="I46">
-        <v>2.3778000000000001</v>
+        <v>943.55</v>
       </c>
       <c r="J46">
-        <v>4.0128000000000004</v>
+        <v>1857.4</v>
       </c>
       <c r="K46">
-        <v>6.3906000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2801</v>
+      </c>
+      <c r="L46">
+        <v>2.5175999999999998</v>
+      </c>
+      <c r="M46">
+        <v>3.7664</v>
+      </c>
+      <c r="N46">
+        <v>6.2839999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="B47">
-        <v>1.9077</v>
+        <v>2.5497000000000001</v>
       </c>
       <c r="C47">
-        <v>1.173E-3</v>
+        <v>1.199E-3</v>
       </c>
       <c r="D47">
-        <v>0.10306999999999999</v>
+        <v>7.7205999999999997E-2</v>
       </c>
       <c r="E47">
-        <v>0.10424</v>
+        <v>7.8405000000000002E-2</v>
       </c>
       <c r="F47">
-        <v>897.7</v>
+        <v>963.7</v>
       </c>
       <c r="G47">
-        <v>1898.5</v>
+        <v>1638.6</v>
       </c>
       <c r="H47">
-        <v>2796.2</v>
+        <v>2602.3000000000002</v>
       </c>
       <c r="I47">
-        <v>2.4247000000000001</v>
+        <v>966.76</v>
       </c>
       <c r="J47">
-        <v>3.9293</v>
+        <v>1835.4</v>
       </c>
       <c r="K47">
-        <v>6.3539000000000003</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2802.2</v>
+      </c>
+      <c r="L47">
+        <v>2.5638999999999998</v>
+      </c>
+      <c r="M47">
+        <v>3.6844000000000001</v>
+      </c>
+      <c r="N47">
+        <v>6.2483000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B48">
-        <v>2.1059999999999999</v>
+        <v>2.7970999999999999</v>
       </c>
       <c r="C48">
-        <v>1.181E-3</v>
+        <v>1.209E-3</v>
       </c>
       <c r="D48">
-        <v>9.3450000000000005E-2</v>
+        <v>7.0295999999999997E-2</v>
       </c>
       <c r="E48">
-        <v>9.4625000000000001E-2</v>
+        <v>7.1504999999999999E-2</v>
       </c>
       <c r="F48">
-        <v>920.6</v>
+        <v>986.76</v>
       </c>
       <c r="G48">
-        <v>1877.6</v>
+        <v>1616.1</v>
       </c>
       <c r="H48">
-        <v>2798.3</v>
+        <v>2602.9</v>
       </c>
       <c r="I48">
-        <v>2.4712999999999998</v>
+        <v>990.14</v>
       </c>
       <c r="J48">
-        <v>3.8462999999999998</v>
+        <v>1812.8</v>
       </c>
       <c r="K48">
-        <v>6.3175999999999997</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2802.9</v>
+      </c>
+      <c r="L48">
+        <v>2.61</v>
+      </c>
+      <c r="M48">
+        <v>3.6027999999999998</v>
+      </c>
+      <c r="N48">
+        <v>6.2127999999999997</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="B49">
-        <v>2.3197999999999999</v>
+        <v>3.0626000000000002</v>
       </c>
       <c r="C49">
-        <v>1.1900000000000001E-3</v>
+        <v>1.219E-3</v>
       </c>
       <c r="D49">
-        <v>8.4849999999999995E-2</v>
+        <v>6.4080999999999999E-2</v>
       </c>
       <c r="E49">
-        <v>8.6038000000000003E-2</v>
+        <v>6.5299999999999997E-2</v>
       </c>
       <c r="F49">
-        <v>943.7</v>
+        <v>1010</v>
       </c>
       <c r="G49">
-        <v>1856.2</v>
+        <v>1593.2</v>
       </c>
       <c r="H49">
-        <v>2799.9</v>
+        <v>2603.1999999999998</v>
       </c>
       <c r="I49">
-        <v>2.5177999999999998</v>
+        <v>1013.7</v>
       </c>
       <c r="J49">
-        <v>3.7639</v>
+        <v>1789.5</v>
       </c>
       <c r="K49">
-        <v>6.2816999999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2803.2</v>
+      </c>
+      <c r="L49">
+        <v>2.6560000000000001</v>
+      </c>
+      <c r="M49">
+        <v>3.5215999999999998</v>
+      </c>
+      <c r="N49">
+        <v>6.1775000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="B50">
-        <v>2.5501</v>
+        <v>3.347</v>
       </c>
       <c r="C50">
-        <v>1.199E-3</v>
+        <v>1.2290000000000001E-3</v>
       </c>
       <c r="D50">
-        <v>7.1150000000000005E-2</v>
+        <v>5.8478000000000002E-2</v>
       </c>
       <c r="E50">
-        <v>7.8349000000000002E-2</v>
+        <v>5.9707000000000003E-2</v>
       </c>
       <c r="F50">
-        <v>966.9</v>
+        <v>1033.4000000000001</v>
       </c>
       <c r="G50">
-        <v>1834.3</v>
+        <v>1569.8</v>
       </c>
       <c r="H50">
-        <v>2801.2</v>
+        <v>2603.1</v>
       </c>
       <c r="I50">
-        <v>2.5640999999999998</v>
+        <v>1037.5</v>
       </c>
       <c r="J50">
-        <v>3.6819999999999999</v>
+        <v>1765.5</v>
       </c>
       <c r="K50">
-        <v>6.2461000000000002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2803</v>
+      </c>
+      <c r="L50">
+        <v>2.7018</v>
+      </c>
+      <c r="M50">
+        <v>3.4405000000000001</v>
+      </c>
+      <c r="N50">
+        <v>6.1424000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="B51">
-        <v>2.7976000000000001</v>
+        <v>3.6511999999999998</v>
       </c>
       <c r="C51">
-        <v>1.209E-3</v>
+        <v>1.24E-3</v>
       </c>
       <c r="D51">
-        <v>7.0239999999999997E-2</v>
+        <v>5.3416000000000012E-2</v>
       </c>
       <c r="E51">
-        <v>7.145E-2</v>
+        <v>5.4656000000000003E-2</v>
       </c>
       <c r="F51">
-        <v>990.3</v>
+        <v>1056.9000000000001</v>
       </c>
       <c r="G51">
-        <v>1811.7</v>
+        <v>1545.7</v>
       </c>
       <c r="H51">
-        <v>2802</v>
+        <v>2602.6999999999998</v>
       </c>
       <c r="I51">
-        <v>2.6101999999999999</v>
+        <v>1061.5</v>
       </c>
       <c r="J51">
-        <v>3.6006</v>
+        <v>1740.8</v>
       </c>
       <c r="K51">
-        <v>6.2107000000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2802.2</v>
+      </c>
+      <c r="L51">
+        <v>2.7475999999999998</v>
+      </c>
+      <c r="M51">
+        <v>3.3595999999999999</v>
+      </c>
+      <c r="N51">
+        <v>6.1071999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="B52">
-        <v>3.0632000000000001</v>
+        <v>3.9762</v>
       </c>
       <c r="C52">
-        <v>1.219E-3</v>
+        <v>1.2520000000000001E-3</v>
       </c>
       <c r="D52">
-        <v>6.402999999999999E-2</v>
+        <v>4.8832999999999988E-2</v>
       </c>
       <c r="E52">
-        <v>6.424500000000001E-2</v>
+        <v>5.0084999999999998E-2</v>
       </c>
       <c r="F52">
-        <v>1013.8</v>
+        <v>1080.7</v>
       </c>
       <c r="G52">
-        <v>1788.5</v>
+        <v>1521.1</v>
       </c>
       <c r="H52">
-        <v>2802.3</v>
+        <v>2601.8000000000002</v>
       </c>
       <c r="I52">
-        <v>2.6560999999999999</v>
+        <v>1085.7</v>
       </c>
       <c r="J52">
-        <v>3.5194000000000001</v>
+        <v>1715.3</v>
       </c>
       <c r="K52">
-        <v>6.1756000000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2801</v>
+      </c>
+      <c r="L52">
+        <v>2.7932999999999999</v>
+      </c>
+      <c r="M52">
+        <v>3.2787999999999999</v>
+      </c>
+      <c r="N52">
+        <v>6.0720999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="B53">
-        <v>3.3477999999999999</v>
+        <v>4.3228999999999997</v>
       </c>
       <c r="C53">
-        <v>1.2290000000000001E-3</v>
+        <v>1.263E-3</v>
       </c>
       <c r="D53">
-        <v>5.8420000000000007E-2</v>
+        <v>4.4678000000000002E-2</v>
       </c>
       <c r="E53">
-        <v>5.9644999999999997E-2</v>
+        <v>4.5941000000000003E-2</v>
       </c>
       <c r="F53">
-        <v>1037.5999999999999</v>
+        <v>1104.7</v>
       </c>
       <c r="G53">
-        <v>1764.6</v>
+        <v>1495.8</v>
       </c>
       <c r="H53">
-        <v>2802.2</v>
+        <v>2600.5</v>
       </c>
       <c r="I53">
-        <v>2.702</v>
+        <v>1110.0999999999999</v>
       </c>
       <c r="J53">
-        <v>3.4386000000000001</v>
+        <v>1689</v>
       </c>
       <c r="K53">
-        <v>6.1406000000000001</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2799.1</v>
+      </c>
+      <c r="L53">
+        <v>2.839</v>
+      </c>
+      <c r="M53">
+        <v>3.1979000000000002</v>
+      </c>
+      <c r="N53">
+        <v>6.0369000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="B54">
-        <v>3.6522999999999999</v>
+        <v>4.6923000000000004</v>
       </c>
       <c r="C54">
-        <v>1.24E-3</v>
+        <v>1.276E-3</v>
       </c>
       <c r="D54">
-        <v>5.1370000000000013E-2</v>
+        <v>4.0898999999999998E-2</v>
       </c>
       <c r="E54">
-        <v>5.4605999999999988E-2</v>
+        <v>4.2174999999999997E-2</v>
       </c>
       <c r="F54">
-        <v>1061.5999999999999</v>
+        <v>1128.8</v>
       </c>
       <c r="G54">
-        <v>1740</v>
+        <v>1469.9</v>
       </c>
       <c r="H54">
-        <v>2801.6</v>
+        <v>2598.6999999999998</v>
       </c>
       <c r="I54">
-        <v>2.7477999999999998</v>
+        <v>1134.8</v>
       </c>
       <c r="J54">
-        <v>3.3578999999999999</v>
+        <v>1661.8</v>
       </c>
       <c r="K54">
-        <v>6.1056999999999997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2796.6</v>
+      </c>
+      <c r="L54">
+        <v>2.8847</v>
+      </c>
+      <c r="M54">
+        <v>3.1168999999999998</v>
+      </c>
+      <c r="N54">
+        <v>6.0016999999999996</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="B55">
-        <v>3.9775999999999998</v>
+        <v>5.0853000000000002</v>
       </c>
       <c r="C55">
-        <v>1.2509999999999999E-3</v>
+        <v>1.289E-3</v>
       </c>
       <c r="D55">
-        <v>4.879E-2</v>
+        <v>3.7458999999999999E-2</v>
       </c>
       <c r="E55">
-        <v>5.0036999999999998E-2</v>
+        <v>3.8747999999999998E-2</v>
       </c>
       <c r="F55">
-        <v>1085.8</v>
+        <v>1153.3</v>
       </c>
       <c r="G55">
-        <v>1714.7</v>
+        <v>1443.2</v>
       </c>
       <c r="H55">
-        <v>2800.4</v>
+        <v>2596.5</v>
       </c>
       <c r="I55">
-        <v>2.7934999999999999</v>
+        <v>1159.8</v>
       </c>
       <c r="J55">
-        <v>3.2772999999999999</v>
+        <v>1633.7</v>
       </c>
       <c r="K55">
-        <v>6.0708000000000002</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2793.5</v>
+      </c>
+      <c r="L55">
+        <v>2.9304000000000001</v>
+      </c>
+      <c r="M55">
+        <v>3.0358000000000001</v>
+      </c>
+      <c r="N55">
+        <v>5.9661999999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="B56">
-        <v>4.3246000000000002</v>
+        <v>5.5030000000000001</v>
       </c>
       <c r="C56">
-        <v>1.263E-3</v>
+        <v>1.3029999999999999E-3</v>
       </c>
       <c r="D56">
-        <v>4.879E-2</v>
+        <v>3.4319000000000002E-2</v>
       </c>
       <c r="E56">
-        <v>4.5895999999999999E-2</v>
+        <v>3.5622000000000001E-2</v>
       </c>
       <c r="F56">
-        <v>1110.2</v>
+        <v>1177.9000000000001</v>
       </c>
       <c r="G56">
-        <v>1688.5</v>
+        <v>1415.7</v>
       </c>
       <c r="H56">
-        <v>2798.7</v>
+        <v>2593.6999999999998</v>
       </c>
       <c r="I56">
-        <v>2.8391999999999999</v>
+        <v>1185.0999999999999</v>
       </c>
       <c r="J56">
-        <v>3.1968000000000001</v>
+        <v>1604.6</v>
       </c>
       <c r="K56">
-        <v>6.0358999999999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2789.7</v>
+      </c>
+      <c r="L56">
+        <v>2.9762</v>
+      </c>
+      <c r="M56">
+        <v>2.9542000000000002</v>
+      </c>
+      <c r="N56">
+        <v>5.9305000000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="B57">
-        <v>4.6943000000000001</v>
+        <v>5.9463999999999997</v>
       </c>
       <c r="C57">
-        <v>1.276E-3</v>
+        <v>1.317E-3</v>
       </c>
       <c r="D57">
-        <v>4.086E-2</v>
+        <v>3.1449999999999999E-2</v>
       </c>
       <c r="E57">
-        <v>4.2130000000000001E-2</v>
+        <v>3.2766999999999998E-2</v>
       </c>
       <c r="F57">
-        <v>1134.9000000000001</v>
+        <v>1202.9000000000001</v>
       </c>
       <c r="G57">
-        <v>1661.5</v>
+        <v>1387.4</v>
       </c>
       <c r="H57">
-        <v>2796.4</v>
+        <v>2590.3000000000002</v>
       </c>
       <c r="I57">
-        <v>2.8847999999999998</v>
+        <v>1210.7</v>
       </c>
       <c r="J57">
-        <v>3.1160999999999999</v>
+        <v>1574.5</v>
       </c>
       <c r="K57">
-        <v>6.0010000000000003</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2785.2</v>
+      </c>
+      <c r="L57">
+        <v>3.0221</v>
+      </c>
+      <c r="M57">
+        <v>2.8723000000000001</v>
+      </c>
+      <c r="N57">
+        <v>5.8944000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="B58">
-        <v>5.0876999999999999</v>
+        <v>6.4166000000000007</v>
       </c>
       <c r="C58">
-        <v>1.289E-3</v>
+        <v>1.333E-3</v>
       </c>
       <c r="D58">
-        <v>3.7429999999999998E-2</v>
+        <v>2.8819999999999998E-2</v>
       </c>
       <c r="E58">
-        <v>3.8710000000000001E-2</v>
+        <v>3.0152999999999999E-2</v>
       </c>
       <c r="F58">
-        <v>1159.9000000000001</v>
+        <v>1228.2</v>
       </c>
       <c r="G58">
-        <v>1633.5</v>
+        <v>1358.2</v>
       </c>
       <c r="H58">
-        <v>2793.5</v>
+        <v>2586.4</v>
       </c>
       <c r="I58">
-        <v>2.9306000000000001</v>
+        <v>1236.7</v>
       </c>
       <c r="J58">
-        <v>3.0352999999999999</v>
+        <v>1543.2</v>
       </c>
       <c r="K58">
-        <v>5.9657999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2779.9</v>
+      </c>
+      <c r="L58">
+        <v>3.0680999999999998</v>
+      </c>
+      <c r="M58">
+        <v>2.7898000000000001</v>
+      </c>
+      <c r="N58">
+        <v>5.8578999999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="B59">
-        <v>5.5057999999999998</v>
+        <v>6.9146000000000001</v>
       </c>
       <c r="C59">
-        <v>1.3029999999999999E-3</v>
+        <v>1.3489999999999999E-3</v>
       </c>
       <c r="D59">
-        <v>3.4290000000000001E-2</v>
+        <v>2.6407E-2</v>
       </c>
       <c r="E59">
-        <v>3.5588000000000002E-2</v>
+        <v>2.7755999999999999E-2</v>
       </c>
       <c r="F59">
-        <v>1185.2</v>
+        <v>1253.7</v>
       </c>
       <c r="G59">
-        <v>1604.6</v>
+        <v>1328.1</v>
       </c>
       <c r="H59">
-        <v>2789.9</v>
+        <v>2581.8000000000002</v>
       </c>
       <c r="I59">
-        <v>2.9763000000000002</v>
+        <v>1263.0999999999999</v>
       </c>
       <c r="J59">
-        <v>2.9540999999999999</v>
+        <v>1510.7</v>
       </c>
       <c r="K59">
-        <v>5.9303999999999997</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2773.7</v>
+      </c>
+      <c r="L59">
+        <v>3.1143999999999998</v>
+      </c>
+      <c r="M59">
+        <v>2.7065999999999999</v>
+      </c>
+      <c r="N59">
+        <v>5.8209999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="B60">
-        <v>5.9496000000000002</v>
+        <v>7.4417999999999997</v>
       </c>
       <c r="C60">
-        <v>1.317E-3</v>
+        <v>1.366E-3</v>
       </c>
       <c r="D60">
-        <v>3.1419999999999997E-2</v>
+        <v>2.4188000000000001E-2</v>
       </c>
       <c r="E60">
-        <v>3.2736000000000001E-2</v>
+        <v>2.5554E-2</v>
       </c>
       <c r="F60">
-        <v>1210.9000000000001</v>
+        <v>1279.7</v>
       </c>
       <c r="G60">
-        <v>1574.7</v>
+        <v>1296.9000000000001</v>
       </c>
       <c r="H60">
-        <v>2785.5</v>
+        <v>2576.5</v>
       </c>
       <c r="I60">
-        <v>3.0222000000000002</v>
+        <v>1289.8</v>
       </c>
       <c r="J60">
-        <v>2.8725000000000001</v>
+        <v>1476.9</v>
       </c>
       <c r="K60">
-        <v>5.8947000000000003</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2766.7</v>
+      </c>
+      <c r="L60">
+        <v>3.1608000000000001</v>
+      </c>
+      <c r="M60">
+        <v>2.6225000000000001</v>
+      </c>
+      <c r="N60">
+        <v>5.7834000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="B61">
-        <v>6.4201999999999986</v>
+        <v>7.9989999999999997</v>
       </c>
       <c r="C61">
-        <v>1.3320000000000001E-3</v>
+        <v>1.384E-3</v>
       </c>
       <c r="D61">
-        <v>2.8799999999999999E-2</v>
+        <v>2.2144E-2</v>
       </c>
       <c r="E61">
-        <v>3.0126E-2</v>
+        <v>2.3528E-2</v>
       </c>
       <c r="F61">
-        <v>1236.8</v>
+        <v>1306</v>
       </c>
       <c r="G61">
-        <v>1543.6</v>
+        <v>1264.5</v>
       </c>
       <c r="H61">
-        <v>2780.4</v>
+        <v>2570.5</v>
       </c>
       <c r="I61">
-        <v>3.0682999999999998</v>
+        <v>1317.1</v>
       </c>
       <c r="J61">
-        <v>2.7902999999999998</v>
+        <v>1441.6</v>
       </c>
       <c r="K61">
-        <v>5.8586</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2758.7</v>
+      </c>
+      <c r="L61">
+        <v>3.2075999999999998</v>
+      </c>
+      <c r="M61">
+        <v>2.5373999999999999</v>
+      </c>
+      <c r="N61">
+        <v>5.7450000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="B62">
-        <v>6.9186000000000014</v>
+        <v>8.5878999999999994</v>
       </c>
       <c r="C62">
-        <v>1.3489999999999999E-3</v>
+        <v>1.4040000000000001E-3</v>
       </c>
       <c r="D62">
-        <v>2.6380000000000001E-2</v>
+        <v>2.0254999999999999E-2</v>
       </c>
       <c r="E62">
-        <v>2.7733000000000001E-2</v>
+        <v>2.1659000000000001E-2</v>
       </c>
       <c r="F62">
-        <v>1263.2</v>
+        <v>1332.7</v>
       </c>
       <c r="G62">
-        <v>1511.3</v>
+        <v>1230.9000000000001</v>
       </c>
       <c r="H62">
-        <v>2774.5</v>
+        <v>2563.6</v>
       </c>
       <c r="I62">
-        <v>3.1145999999999998</v>
+        <v>1344.8</v>
       </c>
       <c r="J62">
-        <v>2.7073999999999998</v>
+        <v>1404.8</v>
       </c>
       <c r="K62">
-        <v>5.8220000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2749.6</v>
+      </c>
+      <c r="L62">
+        <v>3.2547999999999999</v>
+      </c>
+      <c r="M62">
+        <v>2.4510999999999998</v>
+      </c>
+      <c r="N62">
+        <v>5.7058999999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="B63">
-        <v>7.4460999999999986</v>
+        <v>9.2094000000000005</v>
       </c>
       <c r="C63">
-        <v>1.366E-3</v>
+        <v>1.4250000000000001E-3</v>
       </c>
       <c r="D63">
-        <v>2.4170000000000001E-2</v>
+        <v>1.8506999999999999E-2</v>
       </c>
       <c r="E63">
-        <v>2.5534999999999999E-2</v>
+        <v>1.9931999999999998E-2</v>
       </c>
       <c r="F63">
-        <v>1290</v>
+        <v>1360</v>
       </c>
       <c r="G63">
-        <v>1477.6</v>
+        <v>1195.9000000000001</v>
       </c>
       <c r="H63">
-        <v>2767.6</v>
+        <v>2555.8000000000002</v>
       </c>
       <c r="I63">
-        <v>3.1610999999999998</v>
+        <v>1373.1</v>
       </c>
       <c r="J63">
-        <v>2.6236999999999999</v>
+        <v>1366.3</v>
       </c>
       <c r="K63">
-        <v>5.7847999999999997</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2739.4</v>
+      </c>
+      <c r="L63">
+        <v>3.3024</v>
+      </c>
+      <c r="M63">
+        <v>2.3633000000000002</v>
+      </c>
+      <c r="N63">
+        <v>5.6657000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="B64">
-        <v>8.0036999999999985</v>
+        <v>9.8650000000000002</v>
       </c>
       <c r="C64">
-        <v>1.384E-3</v>
+        <v>1.4469999999999999E-3</v>
       </c>
       <c r="D64">
-        <v>2.213E-2</v>
+        <v>1.6886000000000002E-2</v>
       </c>
       <c r="E64">
-        <v>2.3512999999999999E-2</v>
+        <v>1.8332999999999999E-2</v>
       </c>
       <c r="F64">
-        <v>1317.3</v>
+        <v>1387.7</v>
       </c>
       <c r="G64">
-        <v>1442.6</v>
+        <v>1159.3</v>
       </c>
       <c r="H64">
-        <v>2759.8</v>
+        <v>2547.1</v>
       </c>
       <c r="I64">
-        <v>3.2079</v>
+        <v>1402</v>
       </c>
       <c r="J64">
-        <v>2.5388999999999999</v>
+        <v>1325.9</v>
       </c>
       <c r="K64">
-        <v>5.7469000000000001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2727.9</v>
+      </c>
+      <c r="L64">
+        <v>3.3506</v>
+      </c>
+      <c r="M64">
+        <v>2.2736999999999998</v>
+      </c>
+      <c r="N64">
+        <v>5.6242999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="B65">
-        <v>8.5927000000000007</v>
+        <v>10.555999999999999</v>
       </c>
       <c r="C65">
-        <v>1.4040000000000001E-3</v>
+        <v>1.472E-3</v>
       </c>
       <c r="D65">
-        <v>2.0250000000000001E-2</v>
+        <v>1.5377E-2</v>
       </c>
       <c r="E65">
-        <v>2.1649000000000002E-2</v>
+        <v>1.6848999999999999E-2</v>
       </c>
       <c r="F65">
-        <v>1345.1</v>
+        <v>1416.1</v>
       </c>
       <c r="G65">
-        <v>1406</v>
+        <v>1121.0999999999999</v>
       </c>
       <c r="H65">
-        <v>2751</v>
+        <v>2537.1999999999998</v>
       </c>
       <c r="I65">
-        <v>3.2551999999999999</v>
+        <v>1431.6</v>
       </c>
       <c r="J65">
-        <v>2.4529000000000001</v>
+        <v>1283.4000000000001</v>
       </c>
       <c r="K65">
-        <v>5.7081</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2715</v>
+      </c>
+      <c r="L65">
+        <v>3.3994</v>
+      </c>
+      <c r="M65">
+        <v>2.1821000000000002</v>
+      </c>
+      <c r="N65">
+        <v>5.5815999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="B66">
-        <v>9.2143999999999995</v>
+        <v>11.284000000000001</v>
       </c>
       <c r="C66">
-        <v>1.4250000000000001E-3</v>
+        <v>1.4989999999999999E-3</v>
       </c>
       <c r="D66">
-        <v>1.8409999999999999E-2</v>
+        <v>1.3971000000000001E-2</v>
       </c>
       <c r="E66">
-        <v>1.9927E-2</v>
+        <v>1.5469999999999999E-2</v>
       </c>
       <c r="F66">
-        <v>1373.4</v>
+        <v>1445.1</v>
       </c>
       <c r="G66">
-        <v>1367.7</v>
+        <v>1080.9000000000001</v>
       </c>
       <c r="H66">
-        <v>2741.1</v>
+        <v>2526</v>
       </c>
       <c r="I66">
-        <v>3.3029000000000002</v>
+        <v>1462</v>
       </c>
       <c r="J66">
-        <v>2.3656000000000001</v>
+        <v>1238.5</v>
       </c>
       <c r="K66">
-        <v>5.6684999999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2700.6</v>
+      </c>
+      <c r="L66">
+        <v>3.4491000000000001</v>
+      </c>
+      <c r="M66">
+        <v>2.0880999999999998</v>
+      </c>
+      <c r="N66">
+        <v>5.5372000000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="B67">
-        <v>9.870000000000001</v>
+        <v>12.051</v>
       </c>
       <c r="C67">
-        <v>1.4430000000000001E-3</v>
+        <v>1.5280000000000001E-3</v>
       </c>
       <c r="D67">
-        <v>1.6879999999999999E-2</v>
+        <v>1.2655E-2</v>
       </c>
       <c r="E67">
-        <v>1.8334E-2</v>
+        <v>1.4182999999999999E-2</v>
       </c>
       <c r="F67">
-        <v>1402.4</v>
+        <v>1475</v>
       </c>
       <c r="G67">
-        <v>1327.6</v>
+        <v>1038.5</v>
       </c>
       <c r="H67">
-        <v>2730</v>
+        <v>2513.4</v>
       </c>
       <c r="I67">
-        <v>3.3512</v>
+        <v>1493.4</v>
       </c>
       <c r="J67">
-        <v>2.2766000000000002</v>
+        <v>1191</v>
       </c>
       <c r="K67">
-        <v>5.6277999999999997</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2684.3</v>
+      </c>
+      <c r="L67">
+        <v>3.4998</v>
+      </c>
+      <c r="M67">
+        <v>1.9911000000000001</v>
+      </c>
+      <c r="N67">
+        <v>5.4908000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="B68">
-        <v>10.561</v>
+        <v>12.858000000000001</v>
       </c>
       <c r="C68">
-        <v>1.4729999999999999E-3</v>
+        <v>1.56E-3</v>
       </c>
       <c r="D68">
-        <v>1.5089999999999999E-2</v>
+        <v>1.1419E-2</v>
       </c>
       <c r="E68">
-        <v>1.6855999999999999E-2</v>
+        <v>1.2978999999999999E-2</v>
       </c>
       <c r="F68">
-        <v>1432.1</v>
+        <v>1505.7</v>
       </c>
       <c r="G68">
-        <v>1285.5</v>
+        <v>993.5</v>
       </c>
       <c r="H68">
-        <v>2717.6</v>
+        <v>2499.1999999999998</v>
       </c>
       <c r="I68">
-        <v>3.4001999999999999</v>
+        <v>1525.8</v>
       </c>
       <c r="J68">
-        <v>2.1856</v>
+        <v>1140.3</v>
       </c>
       <c r="K68">
-        <v>5.5857999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2666</v>
+      </c>
+      <c r="L68">
+        <v>3.5516000000000001</v>
+      </c>
+      <c r="M68">
+        <v>1.8906000000000001</v>
+      </c>
+      <c r="N68">
+        <v>5.4421999999999997</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="B69">
-        <v>11.289</v>
+        <v>13.707000000000001</v>
       </c>
       <c r="C69">
-        <v>1.5E-3</v>
+        <v>1.5969999999999999E-3</v>
       </c>
       <c r="D69">
-        <v>1.3979999999999999E-2</v>
+        <v>1.0251E-2</v>
       </c>
       <c r="E69">
-        <v>1.5480000000000001E-2</v>
+        <v>1.1847999999999999E-2</v>
       </c>
       <c r="F69">
-        <v>1462.6</v>
+        <v>1537.5</v>
       </c>
       <c r="G69">
-        <v>1241.0999999999999</v>
+        <v>945.5</v>
       </c>
       <c r="H69">
-        <v>2703.7</v>
+        <v>2483</v>
       </c>
       <c r="I69">
-        <v>3.45</v>
+        <v>1559.4</v>
       </c>
       <c r="J69">
-        <v>2.0922999999999998</v>
+        <v>1086</v>
       </c>
       <c r="K69">
-        <v>5.5423</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2645.4</v>
+      </c>
+      <c r="L69">
+        <v>3.605</v>
+      </c>
+      <c r="M69">
+        <v>1.7857000000000001</v>
+      </c>
+      <c r="N69">
+        <v>5.3906999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="B70">
-        <v>12.055999999999999</v>
+        <v>14.601000000000001</v>
       </c>
       <c r="C70">
-        <v>1.529E-3</v>
+        <v>1.6379999999999999E-3</v>
       </c>
       <c r="D70">
-        <v>1.2670000000000001E-2</v>
+        <v>9.1449999999999986E-3</v>
       </c>
       <c r="E70">
-        <v>1.4194999999999999E-2</v>
+        <v>1.0782999999999999E-2</v>
       </c>
       <c r="F70">
-        <v>1494</v>
+        <v>1570.7</v>
       </c>
       <c r="G70">
-        <v>1194</v>
+        <v>893.8</v>
       </c>
       <c r="H70">
-        <v>2688</v>
+        <v>2464.5</v>
       </c>
       <c r="I70">
-        <v>3.5007999999999999</v>
+        <v>1594.6</v>
       </c>
       <c r="J70">
-        <v>1.9961</v>
+        <v>1027.4000000000001</v>
       </c>
       <c r="K70">
-        <v>5.4969000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2622</v>
+      </c>
+      <c r="L70">
+        <v>3.6602000000000001</v>
+      </c>
+      <c r="M70">
+        <v>1.6756</v>
+      </c>
+      <c r="N70">
+        <v>5.3357999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="B71">
-        <v>12.863</v>
+        <v>15.541</v>
       </c>
       <c r="C71">
-        <v>1.562E-3</v>
+        <v>1.6850000000000001E-3</v>
       </c>
       <c r="D71">
-        <v>1.1429999999999999E-2</v>
+        <v>8.0869999999999987E-3</v>
       </c>
       <c r="E71">
-        <v>1.2989000000000001E-2</v>
+        <v>9.7719999999999994E-3</v>
       </c>
       <c r="F71">
-        <v>1526.5</v>
+        <v>1605.5</v>
       </c>
       <c r="G71">
-        <v>1143.5999999999999</v>
+        <v>837.7</v>
       </c>
       <c r="H71">
-        <v>2670.2</v>
+        <v>2443.1999999999998</v>
       </c>
       <c r="I71">
-        <v>3.5528</v>
+        <v>1631.7</v>
       </c>
       <c r="J71">
-        <v>1.8962000000000001</v>
+        <v>963.4</v>
       </c>
       <c r="K71">
-        <v>5.4489999999999998</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2595.1</v>
+      </c>
+      <c r="L71">
+        <v>3.7179000000000002</v>
+      </c>
+      <c r="M71">
+        <v>1.5585</v>
+      </c>
+      <c r="N71">
+        <v>5.2765000000000004</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="B72">
-        <v>13.712</v>
+        <v>16.529</v>
       </c>
       <c r="C72">
-        <v>1.598E-3</v>
+        <v>1.7409999999999999E-3</v>
       </c>
       <c r="D72">
-        <v>1.026E-2</v>
+        <v>7.0650000000000001E-3</v>
       </c>
       <c r="E72">
-        <v>1.1854E-2</v>
+        <v>8.8059999999999996E-3</v>
       </c>
       <c r="F72">
-        <v>1560.3</v>
+        <v>1642.4</v>
       </c>
       <c r="G72">
-        <v>1089.5</v>
+        <v>775.9</v>
       </c>
       <c r="H72">
-        <v>2649.7</v>
+        <v>2418.3000000000002</v>
       </c>
       <c r="I72">
-        <v>3.6063000000000001</v>
+        <v>1671.2</v>
       </c>
       <c r="J72">
-        <v>1.7916000000000001</v>
+        <v>892.7</v>
       </c>
       <c r="K72">
-        <v>5.3978999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2563.9</v>
+      </c>
+      <c r="L72">
+        <v>3.7787999999999999</v>
+      </c>
+      <c r="M72">
+        <v>1.4326000000000001</v>
+      </c>
+      <c r="N72">
+        <v>5.2114000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="B73">
-        <v>14.605</v>
+        <v>17.57</v>
       </c>
       <c r="C73">
-        <v>1.639E-3</v>
+        <v>1.8079999999999999E-3</v>
       </c>
       <c r="D73">
-        <v>9.1400000000000006E-3</v>
+        <v>6.0640000000000008E-3</v>
       </c>
       <c r="E73">
-        <v>1.078E-2</v>
+        <v>7.8720000000000005E-3</v>
       </c>
       <c r="F73">
-        <v>1595.5</v>
+        <v>1682.2</v>
       </c>
       <c r="G73">
-        <v>1030.7</v>
+        <v>706.4</v>
       </c>
       <c r="H73">
-        <v>2626.2</v>
+        <v>2388.6</v>
       </c>
       <c r="I73">
-        <v>3.6616</v>
+        <v>1714</v>
       </c>
       <c r="J73">
-        <v>1.6811</v>
+        <v>812.9</v>
       </c>
       <c r="K73">
-        <v>5.3426999999999998</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2526.9</v>
+      </c>
+      <c r="L73">
+        <v>3.8441999999999998</v>
+      </c>
+      <c r="M73">
+        <v>1.2942</v>
+      </c>
+      <c r="N73">
+        <v>5.1383999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="B74">
-        <v>15.545</v>
+        <v>18.666</v>
       </c>
       <c r="C74">
-        <v>1.686E-3</v>
+        <v>1.895E-3</v>
       </c>
       <c r="D74">
-        <v>8.0700000000000008E-3</v>
+        <v>5.0549999999999996E-3</v>
       </c>
       <c r="E74">
-        <v>9.7629999999999991E-3</v>
+        <v>6.9499999999999996E-3</v>
       </c>
       <c r="F74">
-        <v>1632.5</v>
+        <v>1726.2</v>
       </c>
       <c r="G74">
-        <v>966.4</v>
+        <v>625.70000000000005</v>
       </c>
       <c r="H74">
-        <v>2598.9</v>
+        <v>2351.9</v>
       </c>
       <c r="I74">
-        <v>3.7193000000000001</v>
+        <v>1761.5</v>
       </c>
       <c r="J74">
-        <v>1.5636000000000001</v>
+        <v>720.1</v>
       </c>
       <c r="K74">
-        <v>5.2827999999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2481.6</v>
+      </c>
+      <c r="L74">
+        <v>3.9165000000000001</v>
+      </c>
+      <c r="M74">
+        <v>1.1373</v>
+      </c>
+      <c r="N74">
+        <v>5.0537000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="B75">
-        <v>16.535</v>
+        <v>19.821999999999999</v>
       </c>
       <c r="C75">
-        <v>1.7409999999999999E-3</v>
+        <v>2.0149999999999999E-3</v>
       </c>
       <c r="D75">
-        <v>7.0599999999999986E-3</v>
+        <v>3.9939999999999993E-3</v>
       </c>
       <c r="E75">
-        <v>8.7989999999999995E-3</v>
+        <v>6.0089999999999996E-3</v>
       </c>
       <c r="F75">
-        <v>1671.9</v>
+        <v>1777.2</v>
       </c>
       <c r="G75">
-        <v>895.7</v>
+        <v>526.4</v>
       </c>
       <c r="H75">
-        <v>2567.6999999999998</v>
+        <v>2303.6</v>
       </c>
       <c r="I75">
-        <v>3.78</v>
+        <v>1817.2</v>
       </c>
       <c r="J75">
-        <v>1.4376</v>
+        <v>605.5</v>
       </c>
       <c r="K75">
-        <v>5.2176999999999998</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2422.6999999999998</v>
+      </c>
+      <c r="L75">
+        <v>4.0004</v>
+      </c>
+      <c r="M75">
+        <v>0.94889999999999997</v>
+      </c>
+      <c r="N75">
+        <v>4.9493</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>355</v>
+        <v>370</v>
       </c>
       <c r="B76">
-        <v>17.577000000000002</v>
+        <v>21.044</v>
       </c>
       <c r="C76">
-        <v>1.8090000000000001E-3</v>
+        <v>2.2169999999999998E-3</v>
       </c>
       <c r="D76">
-        <v>6.0499999999999998E-3</v>
+        <v>2.7360000000000002E-3</v>
       </c>
       <c r="E76">
-        <v>7.8589999999999997E-3</v>
+        <v>4.9529999999999999E-3</v>
       </c>
       <c r="F76">
-        <v>1716.6</v>
+        <v>1844.5</v>
       </c>
       <c r="G76">
-        <v>813.8</v>
+        <v>385.6</v>
       </c>
       <c r="H76">
-        <v>2530.4</v>
+        <v>2230.1</v>
       </c>
       <c r="I76">
-        <v>3.8489</v>
+        <v>1891.2</v>
       </c>
       <c r="J76">
-        <v>1.2952999999999999</v>
+        <v>443.1</v>
       </c>
       <c r="K76">
-        <v>5.1441999999999997</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2334.3000000000002</v>
+      </c>
+      <c r="L76">
+        <v>4.1119000000000003</v>
+      </c>
+      <c r="M76">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="N76">
+        <v>4.8009000000000004</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>360</v>
+        <v>373.95</v>
       </c>
       <c r="B77">
-        <v>18.675000000000001</v>
+        <v>22.064</v>
       </c>
       <c r="C77">
-        <v>1.8959999999999999E-3</v>
+        <v>3.1059999999999998E-3</v>
       </c>
       <c r="D77">
-        <v>5.0400000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>6.9389999999999999E-3</v>
+        <v>3.1059999999999998E-3</v>
       </c>
       <c r="F77">
-        <v>1764.2</v>
+        <v>2015.7</v>
       </c>
       <c r="G77">
-        <v>721.3</v>
+        <v>0</v>
       </c>
       <c r="H77">
-        <v>2485.4</v>
+        <v>2015.7</v>
       </c>
       <c r="I77">
-        <v>3.9209999999999998</v>
+        <v>2084.3000000000002</v>
       </c>
       <c r="J77">
-        <v>1.139</v>
+        <v>0</v>
       </c>
       <c r="K77">
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>365</v>
-      </c>
-      <c r="B78">
-        <v>19.832999999999998</v>
-      </c>
-      <c r="C78">
-        <v>2.016E-3</v>
-      </c>
-      <c r="D78">
-        <v>3.9899999999999996E-3</v>
-      </c>
-      <c r="E78">
-        <v>6.0109999999999999E-3</v>
-      </c>
-      <c r="F78">
-        <v>1818</v>
-      </c>
-      <c r="G78">
-        <v>610</v>
-      </c>
-      <c r="H78">
-        <v>2428</v>
-      </c>
-      <c r="I78">
-        <v>4.0021000000000004</v>
-      </c>
-      <c r="J78">
-        <v>0.95579999999999998</v>
-      </c>
-      <c r="K78">
-        <v>4.9579000000000004</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>370</v>
-      </c>
-      <c r="B79">
-        <v>21.053999999999998</v>
-      </c>
-      <c r="C79">
-        <v>2.2139999999999998E-3</v>
-      </c>
-      <c r="D79">
-        <v>2.7599999999999999E-3</v>
-      </c>
-      <c r="E79">
-        <v>4.9719999999999999E-3</v>
-      </c>
-      <c r="F79">
-        <v>1890.2</v>
-      </c>
-      <c r="G79">
-        <v>452.6</v>
-      </c>
-      <c r="H79">
-        <v>2342.8000000000002</v>
-      </c>
-      <c r="I79">
-        <v>4.1108000000000002</v>
-      </c>
-      <c r="J79">
-        <v>0.7036</v>
-      </c>
-      <c r="K79">
-        <v>4.8144</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>374</v>
-      </c>
-      <c r="B80">
-        <v>22.081</v>
-      </c>
-      <c r="C80">
-        <v>2.843E-3</v>
-      </c>
-      <c r="D80">
-        <v>6.3000000000000003E-4</v>
-      </c>
-      <c r="E80">
-        <v>3.4650000000000002E-3</v>
-      </c>
-      <c r="F80">
-        <v>2046.7</v>
-      </c>
-      <c r="G80">
-        <v>109.5</v>
-      </c>
-      <c r="H80">
-        <v>2156.1999999999998</v>
-      </c>
-      <c r="I80">
-        <v>4.3493000000000004</v>
-      </c>
-      <c r="J80">
-        <v>0.16919999999999999</v>
-      </c>
-      <c r="K80">
-        <v>4.5185000000000004</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>374.15</v>
-      </c>
-      <c r="B81">
-        <v>22.12</v>
-      </c>
-      <c r="C81">
-        <v>3.1700000000000001E-3</v>
-      </c>
-      <c r="D81">
+        <v>2084.3000000000002</v>
+      </c>
+      <c r="L77">
+        <v>4.407</v>
+      </c>
+      <c r="M77">
         <v>0</v>
       </c>
-      <c r="E81">
-        <v>3.1700000000000001E-3</v>
-      </c>
-      <c r="F81">
-        <v>2107.4</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>2107.4</v>
-      </c>
-      <c r="I81">
-        <v>4.4428999999999998</v>
-      </c>
-      <c r="J81">
-        <v>0</v>
-      </c>
-      <c r="K81">
-        <v>4.4428999999999998</v>
+      <c r="N77">
+        <v>4.407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>